<commit_message>
update metrics to use proportional scale
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D793D1AB-985E-4477-B25D-57346C7EE1E2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1228,6 +1229,7 @@
         <c:axId val="2129197823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="80"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1278,7 +1280,7 @@
         <c:crossAx val="2122167039"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="20"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2054,6 +2056,7 @@
         <c:axId val="2129197823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6368,8 +6371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="S54" sqref="S54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>